<commit_message>
improved scraper code to find FT odds of bet365
</commit_message>
<xml_diff>
--- a/dixon_coles_model_predictions/_bets.xlsx
+++ b/dixon_coles_model_predictions/_bets.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7265" uniqueCount="943">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7345" uniqueCount="943">
   <si>
     <t>League</t>
   </si>
@@ -3217,11 +3217,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W953"/>
+  <dimension ref="A1:W963"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A933" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A954" sqref="A954"/>
+      <pane ySplit="1" topLeftCell="A942" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A964" sqref="A964"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -73561,6 +73561,716 @@
         <v>0.33</v>
       </c>
     </row>
+    <row r="954" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A954" t="s">
+        <v>882</v>
+      </c>
+      <c r="B954" t="s">
+        <v>917</v>
+      </c>
+      <c r="C954" t="s">
+        <v>887</v>
+      </c>
+      <c r="D954" t="s">
+        <v>25</v>
+      </c>
+      <c r="E954">
+        <v>64.789999999999992</v>
+      </c>
+      <c r="F954">
+        <v>2</v>
+      </c>
+      <c r="G954">
+        <v>0.46</v>
+      </c>
+      <c r="H954" t="s">
+        <v>22</v>
+      </c>
+      <c r="I954" s="2">
+        <v>89.6</v>
+      </c>
+      <c r="J954">
+        <v>1.17</v>
+      </c>
+      <c r="K954">
+        <v>0.05</v>
+      </c>
+      <c r="L954" t="s">
+        <v>28</v>
+      </c>
+      <c r="M954">
+        <v>58.61</v>
+      </c>
+      <c r="N954">
+        <v>1.65</v>
+      </c>
+      <c r="O954">
+        <v>-0.06</v>
+      </c>
+      <c r="P954" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q954">
+        <v>66.210000000000008</v>
+      </c>
+      <c r="R954">
+        <v>1.92</v>
+      </c>
+      <c r="S954">
+        <v>0.41</v>
+      </c>
+      <c r="T954" t="s">
+        <v>25</v>
+      </c>
+      <c r="U954">
+        <v>64.789999999999992</v>
+      </c>
+      <c r="V954">
+        <v>2</v>
+      </c>
+      <c r="W954">
+        <v>0.46</v>
+      </c>
+    </row>
+    <row r="955" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A955" t="s">
+        <v>882</v>
+      </c>
+      <c r="B955" t="s">
+        <v>884</v>
+      </c>
+      <c r="C955" t="s">
+        <v>885</v>
+      </c>
+      <c r="D955" t="s">
+        <v>29</v>
+      </c>
+      <c r="E955">
+        <v>72.52</v>
+      </c>
+      <c r="F955">
+        <v>2.23</v>
+      </c>
+      <c r="G955">
+        <v>0.85</v>
+      </c>
+      <c r="H955" t="s">
+        <v>22</v>
+      </c>
+      <c r="I955">
+        <v>79.72999999999999</v>
+      </c>
+      <c r="J955">
+        <v>1.35</v>
+      </c>
+      <c r="K955">
+        <v>0.1</v>
+      </c>
+      <c r="L955" t="s">
+        <v>28</v>
+      </c>
+      <c r="M955">
+        <v>56.51</v>
+      </c>
+      <c r="N955">
+        <v>2.4300000000000002</v>
+      </c>
+      <c r="O955">
+        <v>0.66</v>
+      </c>
+      <c r="P955" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q955">
+        <v>72.52</v>
+      </c>
+      <c r="R955">
+        <v>2.23</v>
+      </c>
+      <c r="S955">
+        <v>0.85</v>
+      </c>
+      <c r="T955" t="s">
+        <v>15</v>
+      </c>
+      <c r="U955">
+        <v>70.36</v>
+      </c>
+      <c r="V955">
+        <v>1.93</v>
+      </c>
+      <c r="W955">
+        <v>0.51</v>
+      </c>
+    </row>
+    <row r="956" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A956" t="s">
+        <v>882</v>
+      </c>
+      <c r="B956" t="s">
+        <v>888</v>
+      </c>
+      <c r="C956" t="s">
+        <v>942</v>
+      </c>
+      <c r="D956" t="s">
+        <v>33</v>
+      </c>
+      <c r="E956">
+        <v>55.03</v>
+      </c>
+      <c r="F956">
+        <v>2.95</v>
+      </c>
+      <c r="G956">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="H956" t="s">
+        <v>32</v>
+      </c>
+      <c r="I956" s="2">
+        <v>81.7</v>
+      </c>
+      <c r="J956">
+        <v>1.52</v>
+      </c>
+      <c r="K956">
+        <v>0.3</v>
+      </c>
+      <c r="L956" t="s">
+        <v>33</v>
+      </c>
+      <c r="M956">
+        <v>55.03</v>
+      </c>
+      <c r="N956">
+        <v>2.95</v>
+      </c>
+      <c r="O956">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="P956" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q956">
+        <v>59.65</v>
+      </c>
+      <c r="R956">
+        <v>2.08</v>
+      </c>
+      <c r="S956">
+        <v>0.4</v>
+      </c>
+      <c r="T956" t="s">
+        <v>15</v>
+      </c>
+      <c r="U956">
+        <v>60.3</v>
+      </c>
+      <c r="V956">
+        <v>1.84</v>
+      </c>
+      <c r="W956">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="957" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A957" t="s">
+        <v>882</v>
+      </c>
+      <c r="B957" t="s">
+        <v>921</v>
+      </c>
+      <c r="C957" t="s">
+        <v>916</v>
+      </c>
+      <c r="D957" t="s">
+        <v>33</v>
+      </c>
+      <c r="E957">
+        <v>47.15</v>
+      </c>
+      <c r="F957">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="G957">
+        <v>1.98</v>
+      </c>
+      <c r="H957" t="s">
+        <v>32</v>
+      </c>
+      <c r="I957" s="2">
+        <v>86.32</v>
+      </c>
+      <c r="J957">
+        <v>1.88</v>
+      </c>
+      <c r="K957">
+        <v>0.72</v>
+      </c>
+      <c r="L957" t="s">
+        <v>33</v>
+      </c>
+      <c r="M957">
+        <v>47.15</v>
+      </c>
+      <c r="N957">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="O957">
+        <v>1.98</v>
+      </c>
+      <c r="P957" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q957">
+        <v>79.58</v>
+      </c>
+      <c r="R957">
+        <v>1.68</v>
+      </c>
+      <c r="S957">
+        <v>0.42</v>
+      </c>
+      <c r="T957" t="s">
+        <v>25</v>
+      </c>
+      <c r="U957">
+        <v>72.12</v>
+      </c>
+      <c r="V957">
+        <v>1.86</v>
+      </c>
+      <c r="W957">
+        <v>0.47</v>
+      </c>
+    </row>
+    <row r="958" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A958" t="s">
+        <v>620</v>
+      </c>
+      <c r="B958" t="s">
+        <v>621</v>
+      </c>
+      <c r="C958" t="s">
+        <v>673</v>
+      </c>
+      <c r="D958" t="s">
+        <v>29</v>
+      </c>
+      <c r="E958">
+        <v>77.53</v>
+      </c>
+      <c r="F958">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="G958">
+        <v>0.99</v>
+      </c>
+      <c r="H958" t="s">
+        <v>64</v>
+      </c>
+      <c r="I958" s="2">
+        <v>89.38</v>
+      </c>
+      <c r="J958">
+        <v>1.37</v>
+      </c>
+      <c r="K958">
+        <v>0.25</v>
+      </c>
+      <c r="L958" t="s">
+        <v>28</v>
+      </c>
+      <c r="M958">
+        <v>75.45</v>
+      </c>
+      <c r="N958">
+        <v>2.23</v>
+      </c>
+      <c r="O958">
+        <v>0.9</v>
+      </c>
+      <c r="P958" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q958">
+        <v>77.53</v>
+      </c>
+      <c r="R958">
+        <v>2.2799999999999998</v>
+      </c>
+      <c r="S958">
+        <v>0.99</v>
+      </c>
+      <c r="T958" t="s">
+        <v>15</v>
+      </c>
+      <c r="U958">
+        <v>62.89</v>
+      </c>
+      <c r="V958">
+        <v>1.9</v>
+      </c>
+      <c r="W958">
+        <v>0.31</v>
+      </c>
+    </row>
+    <row r="959" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A959" t="s">
+        <v>620</v>
+      </c>
+      <c r="B959" t="s">
+        <v>66</v>
+      </c>
+      <c r="C959" t="s">
+        <v>458</v>
+      </c>
+      <c r="D959" t="s">
+        <v>64</v>
+      </c>
+      <c r="E959" s="2">
+        <v>84.09</v>
+      </c>
+      <c r="F959">
+        <v>1.26</v>
+      </c>
+      <c r="G959">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="H959" t="s">
+        <v>64</v>
+      </c>
+      <c r="I959" s="2">
+        <v>84.09</v>
+      </c>
+      <c r="J959">
+        <v>1.26</v>
+      </c>
+      <c r="K959">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="L959" t="s">
+        <v>28</v>
+      </c>
+      <c r="M959">
+        <v>42.5</v>
+      </c>
+      <c r="N959">
+        <v>1.9</v>
+      </c>
+      <c r="O959">
+        <v>-0.45</v>
+      </c>
+      <c r="P959" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q959">
+        <v>62.06</v>
+      </c>
+      <c r="R959">
+        <v>1.58</v>
+      </c>
+      <c r="S959">
+        <v>-0.03</v>
+      </c>
+      <c r="T959" t="s">
+        <v>15</v>
+      </c>
+      <c r="U959">
+        <v>59.98</v>
+      </c>
+      <c r="V959">
+        <v>1.5</v>
+      </c>
+      <c r="W959">
+        <v>-0.17</v>
+      </c>
+    </row>
+    <row r="960" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A960" t="s">
+        <v>620</v>
+      </c>
+      <c r="B960" t="s">
+        <v>456</v>
+      </c>
+      <c r="C960" t="s">
+        <v>69</v>
+      </c>
+      <c r="D960" t="s">
+        <v>33</v>
+      </c>
+      <c r="E960">
+        <v>43.34</v>
+      </c>
+      <c r="F960">
+        <v>3.15</v>
+      </c>
+      <c r="G960">
+        <v>0.84</v>
+      </c>
+      <c r="H960" t="s">
+        <v>64</v>
+      </c>
+      <c r="I960">
+        <v>79.38</v>
+      </c>
+      <c r="J960">
+        <v>1.32</v>
+      </c>
+      <c r="K960">
+        <v>0.06</v>
+      </c>
+      <c r="L960" t="s">
+        <v>33</v>
+      </c>
+      <c r="M960">
+        <v>43.34</v>
+      </c>
+      <c r="N960">
+        <v>3.15</v>
+      </c>
+      <c r="O960">
+        <v>0.84</v>
+      </c>
+      <c r="P960" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q960">
+        <v>66.44</v>
+      </c>
+      <c r="R960">
+        <v>1.71</v>
+      </c>
+      <c r="S960">
+        <v>0.2</v>
+      </c>
+      <c r="T960" t="s">
+        <v>25</v>
+      </c>
+      <c r="U960">
+        <v>64.02000000000001</v>
+      </c>
+      <c r="V960">
+        <v>1.96</v>
+      </c>
+      <c r="W960">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="961" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A961" t="s">
+        <v>620</v>
+      </c>
+      <c r="B961" t="s">
+        <v>454</v>
+      </c>
+      <c r="C961" t="s">
+        <v>68</v>
+      </c>
+      <c r="D961" t="s">
+        <v>24</v>
+      </c>
+      <c r="E961" s="2">
+        <v>94.98</v>
+      </c>
+      <c r="F961">
+        <v>2.12</v>
+      </c>
+      <c r="G961">
+        <v>1.07</v>
+      </c>
+      <c r="H961" t="s">
+        <v>32</v>
+      </c>
+      <c r="I961">
+        <v>75.319999999999993</v>
+      </c>
+      <c r="J961">
+        <v>1.58</v>
+      </c>
+      <c r="K961">
+        <v>0.25</v>
+      </c>
+      <c r="L961" t="s">
+        <v>23</v>
+      </c>
+      <c r="M961">
+        <v>46.46</v>
+      </c>
+      <c r="N961">
+        <v>2.8</v>
+      </c>
+      <c r="O961">
+        <v>0.65</v>
+      </c>
+      <c r="P961" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q961" s="2">
+        <v>94.98</v>
+      </c>
+      <c r="R961">
+        <v>2.12</v>
+      </c>
+      <c r="S961">
+        <v>1.07</v>
+      </c>
+      <c r="T961" t="s">
+        <v>25</v>
+      </c>
+      <c r="U961" s="2">
+        <v>91.42</v>
+      </c>
+      <c r="V961">
+        <v>1.49</v>
+      </c>
+      <c r="W961">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="962" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A962" t="s">
+        <v>620</v>
+      </c>
+      <c r="B962" t="s">
+        <v>295</v>
+      </c>
+      <c r="C962" t="s">
+        <v>937</v>
+      </c>
+      <c r="D962" t="s">
+        <v>29</v>
+      </c>
+      <c r="E962">
+        <v>71.58</v>
+      </c>
+      <c r="F962">
+        <v>1.95</v>
+      </c>
+      <c r="G962">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H962" t="s">
+        <v>64</v>
+      </c>
+      <c r="I962" s="2">
+        <v>84.51</v>
+      </c>
+      <c r="J962">
+        <v>1.3</v>
+      </c>
+      <c r="K962">
+        <v>0.12</v>
+      </c>
+      <c r="L962" t="s">
+        <v>28</v>
+      </c>
+      <c r="M962">
+        <v>44.81</v>
+      </c>
+      <c r="N962">
+        <v>2.08</v>
+      </c>
+      <c r="O962">
+        <v>-0.15</v>
+      </c>
+      <c r="P962" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q962">
+        <v>71.58</v>
+      </c>
+      <c r="R962">
+        <v>1.95</v>
+      </c>
+      <c r="S962">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="T962" t="s">
+        <v>15</v>
+      </c>
+      <c r="U962">
+        <v>68.03</v>
+      </c>
+      <c r="V962">
+        <v>1.76</v>
+      </c>
+      <c r="W962">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="963" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="A963" t="s">
+        <v>620</v>
+      </c>
+      <c r="B963" t="s">
+        <v>67</v>
+      </c>
+      <c r="C963" t="s">
+        <v>674</v>
+      </c>
+      <c r="D963" t="s">
+        <v>25</v>
+      </c>
+      <c r="E963">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="F963">
+        <v>1.87</v>
+      </c>
+      <c r="G963">
+        <v>0.33</v>
+      </c>
+      <c r="H963" t="s">
+        <v>64</v>
+      </c>
+      <c r="I963" s="2">
+        <v>80.150000000000006</v>
+      </c>
+      <c r="J963">
+        <v>1.35</v>
+      </c>
+      <c r="K963">
+        <v>0.1</v>
+      </c>
+      <c r="L963" t="s">
+        <v>28</v>
+      </c>
+      <c r="M963">
+        <v>51.93</v>
+      </c>
+      <c r="N963">
+        <v>1.98</v>
+      </c>
+      <c r="O963">
+        <v>0.05</v>
+      </c>
+      <c r="P963" t="s">
+        <v>24</v>
+      </c>
+      <c r="Q963">
+        <v>65.72</v>
+      </c>
+      <c r="R963">
+        <v>1.62</v>
+      </c>
+      <c r="S963">
+        <v>0.1</v>
+      </c>
+      <c r="T963" t="s">
+        <v>25</v>
+      </c>
+      <c r="U963">
+        <v>64.930000000000007</v>
+      </c>
+      <c r="V963">
+        <v>1.87</v>
+      </c>
+      <c r="W963">
+        <v>0.33</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>